<commit_message>
modified modules watershed 4
</commit_message>
<xml_diff>
--- a/rnn/gain_new3/data/han/방사성/의암댐_2016.xlsx
+++ b/rnn/gain_new3/data/han/방사성/의암댐_2016.xlsx
@@ -1,25 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\사업관련\환경AI\모듈작업\water-quality-main\water-quality-main\gain_new3\han\방사성\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>year</t>
   </si>
@@ -121,6 +114,9 @@
   </si>
   <si>
     <t>iem_iod_131_dnsty_flag</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
   <si>
     <t>상반기</t>
@@ -150,30 +146,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -191,38 +180,23 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -231,10 +205,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -480,61 +454,55 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.71" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.57" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.71" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.57" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.43" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.43" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.71" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.43" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.43" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.43" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.71" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.71" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.29" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.29" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.29" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.43" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="24" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,18 +606,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>42370</v>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -661,30 +629,30 @@
         <v>127.675555</v>
       </c>
       <c r="AA2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>42491</v>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -696,21 +664,19 @@
         <v>127.675555</v>
       </c>
       <c r="AA3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AB3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AC3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD3">
         <v>1</v>
       </c>
     </row>
+    <row r="4"/>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>